<commit_message>
working oops version - add data only
</commit_message>
<xml_diff>
--- a/sampleinfo.xlsx
+++ b/sampleinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\sqlpy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A64ABC6-C2C0-464F-B2D8-49E500AB30EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2770C601-C897-4CAE-B939-2B244463A458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="3030" windowWidth="21585" windowHeight="11385" xr2:uid="{F1E0DD96-5E13-406D-9160-5CE5C5F9F98D}"/>
+    <workbookView xWindow="4500" yWindow="3480" windowWidth="21585" windowHeight="11385" xr2:uid="{F1E0DD96-5E13-406D-9160-5CE5C5F9F98D}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -66,46 +66,64 @@
     <t>portalpass</t>
   </si>
   <si>
-    <t>Naruto Uzumaki</t>
-  </si>
-  <si>
-    <t>Kakashi Hatake</t>
-  </si>
-  <si>
-    <t>ASTM2859VF</t>
-  </si>
-  <si>
-    <t>BFGR8939GY</t>
-  </si>
-  <si>
-    <t>25th Street</t>
-  </si>
-  <si>
-    <t>2B</t>
-  </si>
-  <si>
-    <t>Jonin area</t>
-  </si>
-  <si>
-    <t>Konoha</t>
-  </si>
-  <si>
-    <t>Fire</t>
-  </si>
-  <si>
     <t>abcdrt</t>
   </si>
   <si>
     <t>djfhtedpdk</t>
   </si>
   <si>
-    <t>1st Street</t>
-  </si>
-  <si>
-    <t>Genin area</t>
-  </si>
-  <si>
-    <t>1A</t>
+    <t>Harry Ried</t>
+  </si>
+  <si>
+    <t>Adolf Mueller</t>
+  </si>
+  <si>
+    <t>CDBC4565AS</t>
+  </si>
+  <si>
+    <t>ERTY7831WD</t>
+  </si>
+  <si>
+    <t>Karen Reed</t>
+  </si>
+  <si>
+    <t>VBDG8932JK</t>
+  </si>
+  <si>
+    <t>74th Street</t>
+  </si>
+  <si>
+    <t>4th Street</t>
+  </si>
+  <si>
+    <t>Peking nagar</t>
+  </si>
+  <si>
+    <t>Urban county</t>
+  </si>
+  <si>
+    <t>Moonbase</t>
+  </si>
+  <si>
+    <t>Marsbase</t>
+  </si>
+  <si>
+    <t>Ontairo</t>
+  </si>
+  <si>
+    <t>Kemp</t>
+  </si>
+  <si>
+    <t>56th Street</t>
+  </si>
+  <si>
+    <t>Rural county</t>
+  </si>
+  <si>
+    <t>Ergocenter</t>
+  </si>
+  <si>
+    <t>gfkhasgka</t>
   </si>
 </sst>
 </file>
@@ -457,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEB0334-4CE1-4C5C-BF63-29E8F51D004F}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,66 +525,95 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2">
+        <v>456123</v>
+      </c>
+      <c r="J2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2">
-        <v>254657</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3">
+        <v>487612</v>
+      </c>
+      <c r="J3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
-        <v>65</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="G3" t="s">
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3">
-        <v>756329</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
+      <c r="C4">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4">
+        <v>125753</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more sample data
</commit_message>
<xml_diff>
--- a/sampleinfo.xlsx
+++ b/sampleinfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\sqlpy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2770C601-C897-4CAE-B939-2B244463A458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEB6A8C-138C-4D04-BC04-BC0A3D9729D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="3480" windowWidth="21585" windowHeight="11385" xr2:uid="{F1E0DD96-5E13-406D-9160-5CE5C5F9F98D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>name</t>
   </si>
@@ -124,6 +124,30 @@
   </si>
   <si>
     <t>gfkhasgka</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>Mary Antonette</t>
+  </si>
+  <si>
+    <t>ASDJ5612GJ</t>
+  </si>
+  <si>
+    <t>80th Street East</t>
+  </si>
+  <si>
+    <t>City centre</t>
+  </si>
+  <si>
+    <t>Vladivostock</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>gfkuavlk2</t>
   </si>
 </sst>
 </file>
@@ -475,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEB0334-4CE1-4C5C-BF63-29E8F51D004F}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,13 +555,10 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
-      </c>
-      <c r="E2">
-        <v>61</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
@@ -563,10 +584,13 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
       </c>
       <c r="F3" t="s">
         <v>21</v>
@@ -614,6 +638,35 @@
       </c>
       <c r="J4" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5">
+        <v>124654</v>
+      </c>
+      <c r="J5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change input data format
</commit_message>
<xml_diff>
--- a/sampleinfo.xlsx
+++ b/sampleinfo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\sqlpy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEB6A8C-138C-4D04-BC04-BC0A3D9729D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACDC826-74B6-48E5-B48F-EEE4C1E43EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="3480" windowWidth="21585" windowHeight="11385" xr2:uid="{F1E0DD96-5E13-406D-9160-5CE5C5F9F98D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>name</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>gfkuavlk2</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>aadhaar</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -499,174 +511,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEB0334-4CE1-4C5C-BF63-29E8F51D004F}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="C2">
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
         <v>24</v>
       </c>
-      <c r="I2">
+      <c r="N2">
         <v>456123</v>
       </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="C3">
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
+      <c r="I3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="J3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
+      <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
+      <c r="M3" t="s">
         <v>25</v>
       </c>
-      <c r="I3">
+      <c r="N3">
         <v>487612</v>
       </c>
-      <c r="J3" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="C4">
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4">
         <v>78</v>
       </c>
-      <c r="D4" t="s">
+      <c r="I4" t="s">
         <v>26</v>
       </c>
-      <c r="E4">
+      <c r="J4">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
+      <c r="K4" t="s">
         <v>27</v>
       </c>
-      <c r="G4" t="s">
+      <c r="L4" t="s">
         <v>28</v>
       </c>
-      <c r="H4" t="s">
+      <c r="M4" t="s">
         <v>25</v>
       </c>
-      <c r="I4">
+      <c r="N4">
         <v>125753</v>
       </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>32</v>
       </c>
-      <c r="C5">
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5">
         <v>47</v>
       </c>
-      <c r="D5" t="s">
+      <c r="I5" t="s">
         <v>33</v>
       </c>
-      <c r="F5" t="s">
+      <c r="K5" t="s">
         <v>34</v>
       </c>
-      <c r="G5" t="s">
+      <c r="L5" t="s">
         <v>35</v>
       </c>
-      <c r="H5" t="s">
+      <c r="M5" t="s">
         <v>36</v>
       </c>
-      <c r="I5">
+      <c r="N5">
         <v>124654</v>
-      </c>
-      <c r="J5" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sample information to be loaded to db
</commit_message>
<xml_diff>
--- a/sampleinfo.xlsx
+++ b/sampleinfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shyam\Documents\sqlpy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACDC826-74B6-48E5-B48F-EEE4C1E43EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB5A868-E8E8-4E87-B338-773BE3690695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="3480" windowWidth="21585" windowHeight="11385" xr2:uid="{F1E0DD96-5E13-406D-9160-5CE5C5F9F98D}"/>
   </bookViews>
@@ -514,12 +514,13 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
@@ -575,6 +576,9 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
+      <c r="B2">
+        <v>4154654879</v>
+      </c>
       <c r="D2" t="s">
         <v>14</v>
       </c>
@@ -604,6 +608,9 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
+      <c r="B3">
+        <v>4167329486</v>
+      </c>
       <c r="D3" t="s">
         <v>15</v>
       </c>
@@ -636,6 +643,9 @@
       <c r="A4" t="s">
         <v>16</v>
       </c>
+      <c r="B4">
+        <v>3068815942</v>
+      </c>
       <c r="D4" t="s">
         <v>17</v>
       </c>
@@ -667,6 +677,9 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
+      </c>
+      <c r="B5">
+        <v>4025176530</v>
       </c>
       <c r="D5" t="s">
         <v>32</v>

</xml_diff>